<commit_message>
Feat: NA for loan installment features
</commit_message>
<xml_diff>
--- a/DS-Project_data-dict/LCdatadictionary.xlsx
+++ b/DS-Project_data-dict/LCdatadictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jujou/Documents/Repos/GRP-6_DS-Project/DS-Project_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jujou/Documents/Repos/GRP-6_DS-Project/DS-Project_data-dict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC974E5-ED71-774C-8951-6315E99E788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415E2302-A468-D345-98D1-18508EFD031E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="22960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="19480" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -2001,8 +2001,8 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3859,6 +3859,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b4a7e659-09bd-4686-945b-72100c560ea7" xsi:nil="true"/>
@@ -3867,15 +3876,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4122,6 +4122,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79FDEF13-2353-4E2A-91F6-5002A8B1DB5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E045B5B-9298-4CA2-B8A8-8516AD835D96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4134,14 +4142,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="b4a7e659-09bd-4686-945b-72100c560ea7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79FDEF13-2353-4E2A-91F6-5002A8B1DB5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>